<commit_message>
0.0.16: Not import myself for recursive definitions.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9573E5-9902-AD4B-82F3-FA08086FA65C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B615E762-16DB-EC48-9E2A-513EECC17A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9100" yWindow="6000" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>クラス名</t>
   </si>
@@ -224,6 +224,50 @@
   </si>
   <si>
     <t>○</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>recursiveParam</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>new SimpleSample()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>再帰</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">サイキ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>import文の自動生成</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t xml:space="preserve">ジドウセイセイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>/* TypeScript 独自。blancoで一括生成されたクラスについて、import文を自動生成します。 */</t>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">ドクジ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">イッカツ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="47" eb="51">
+      <t xml:space="preserve">ジドウセイセイ </t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -719,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -811,19 +855,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1235,10 +1285,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1252,7 +1302,7 @@
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19">
+    <row r="1" spans="1:13" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1260,17 +1310,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1278,9 +1328,9 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="53"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="F5" s="51"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1290,10 +1340,10 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="54"/>
+      <c r="F6" s="52"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1303,10 +1353,10 @@
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="54"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1321,7 +1371,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1336,7 +1386,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:11" s="34" customFormat="1">
+    <row r="10" spans="1:13" s="34" customFormat="1">
       <c r="A10" s="40" t="s">
         <v>26</v>
       </c>
@@ -1350,7 +1400,7 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:11" s="34" customFormat="1">
+    <row r="11" spans="1:13" s="34" customFormat="1">
       <c r="A11" s="40" t="s">
         <v>28</v>
       </c>
@@ -1364,213 +1414,245 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="31" t="s">
+    <row r="12" spans="1:13" s="34" customFormat="1">
+      <c r="A12" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="3" t="s">
+    <row r="15" spans="1:13">
+      <c r="A15" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A17" s="52" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A18" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B18" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C18" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D18" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E18" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F18" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G18" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="51"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="15"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="29"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21" t="s">
-        <v>40</v>
-      </c>
+      <c r="E20" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="21"/>
       <c r="G20" s="21" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
+      <c r="J20" s="29"/>
       <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="19">
+        <v>2</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="F21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="23"/>
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
+      <c r="A22" s="19">
+        <v>3</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="E22" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
+      <c r="G22" s="21" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="23"/>
       <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="28"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23"/>
       <c r="K23" s="15"/>
     </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G17:H18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
+  <mergeCells count="8">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G18:H19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:F39" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E40:F40" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{9B350086-4234-7F42-90E1-E9696B21763F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C12" xr:uid="{9B350086-4234-7F42-90E1-E9696B21763F}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{37676737-95C3-434E-BC4C-270691A9AC5F}">

</xml_diff>

<commit_message>
0.1.4: create toJSON for extended classes.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B615E762-16DB-EC48-9E2A-513EECC17A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B9372A-3090-6A43-B25E-F62445328714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9100" yWindow="6000" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15000" yWindow="2280" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -857,6 +857,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -868,12 +874,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1415,10 +1415,10 @@
       <c r="H11"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="58"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="42" t="s">
         <v>27</v>
       </c>
@@ -1501,41 +1501,41 @@
       <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="53"/>
+      <c r="H18" s="55"/>
       <c r="I18" s="16"/>
       <c r="J18" s="17"/>
       <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
       <c r="I19" s="18"/>
       <c r="J19" s="30"/>
       <c r="K19" s="15"/>

</xml_diff>

<commit_message>
3.0.7 adapt "パッケージ(Ts)" column on definition sheet.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B9372A-3090-6A43-B25E-F62445328714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3467F4A2-05B3-B54F-9301-17F057737D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15000" yWindow="2280" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>クラス名</t>
   </si>
@@ -268,6 +268,14 @@
     <rPh sb="47" eb="51">
       <t xml:space="preserve">ジドウセイセイ </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>パッケージ(Ts)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blanco.sample.valueobjectts.typescript</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -763,27 +771,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,24 +802,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -825,15 +831,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -855,24 +859,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1285,10 +1289,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1328,7 +1332,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="51"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
@@ -1340,7 +1344,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="52"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:13">
@@ -1351,33 +1355,31 @@
       <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="52"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="8"/>
+      <c r="C8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -1386,27 +1388,28 @@
       <c r="H9" s="12"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:13" s="34" customFormat="1">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="39" t="s">
         <v>27</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:13" s="34" customFormat="1">
-      <c r="A11" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="42" t="s">
-        <v>40</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1414,248 +1417,254 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:13" s="34" customFormat="1">
-      <c r="A12" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
+    <row r="12" spans="1:13">
+      <c r="A12" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="50"/>
+      <c r="C13" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="31" t="s">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="35" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="3" t="s">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A18" s="56" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A19" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B19" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C19" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D19" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E19" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="F19" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="55" t="s">
+      <c r="G19" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="55"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="56"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="15"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="19">
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="18">
         <v>1</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21" t="s">
+      <c r="F21" s="20"/>
+      <c r="G21" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="19">
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="18">
         <v>2</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G22" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="19">
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="18">
         <v>3</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21" t="s">
+      <c r="F23" s="20"/>
+      <c r="G23" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="15"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="15"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="G18:H19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="G19:H20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E40:F40" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E41:F41" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C12" xr:uid="{9B350086-4234-7F42-90E1-E9696B21763F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C13" xr:uid="{9B350086-4234-7F42-90E1-E9696B21763F}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{37676737-95C3-434E-BC4C-270691A9AC5F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{37676737-95C3-434E-BC4C-270691A9AC5F}">
       <formula1>createToString</formula1>
     </dataValidation>
   </dataValidations>
@@ -1690,65 +1699,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="44"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="41" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="46"/>
-      <c r="D4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="45" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="50"/>
+      <c r="B6" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>